<commit_message>
exc2 fill part of questions
</commit_message>
<xml_diff>
--- a/Exc2/checklist.xlsx
+++ b/Exc2/checklist.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
   <si>
     <t>№</t>
   </si>
@@ -52,15 +52,27 @@
     <t>Используются ли системы аутентификации пользователей для доступа к системам?</t>
   </si>
   <si>
+    <t>да</t>
+  </si>
+  <si>
+    <t>Есть auth-service - Keycloak</t>
+  </si>
+  <si>
     <t>Созданы ли замкнутые контуры для подсистем, работающих с чувствительными данными?</t>
   </si>
   <si>
     <t>Ограничен ли доступ к системам из внешних источников?</t>
   </si>
   <si>
+    <t>доступ идет через firewall, но не известно насколько полностью ограничен</t>
+  </si>
+  <si>
     <t>Ведётся ли единый реестр учётных записей?</t>
   </si>
   <si>
+    <t>keycloak</t>
+  </si>
+  <si>
     <t>Используются ли средства управления учётными записями на базе единого реестра?</t>
   </si>
   <si>
@@ -158,6 +170,9 @@
   </si>
   <si>
     <t>Используется ли межсетевой экран для ограничения входящего и исходящего трафика?</t>
+  </si>
+  <si>
+    <t>некйий firewall есть, но настройки не известны</t>
   </si>
   <si>
     <t>Реализована ли сегментация сети на логические зоны (DMZ, корпоративная сеть, гостевая сеть) для ограничения доступа к критическим ресурсам?</t>
@@ -295,18 +310,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -327,6 +342,19 @@
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -366,13 +394,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -382,38 +434,59 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,8 +506,9 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffe7e6e6"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffd9e2f3"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffe2eeda"/>
     </indexedColors>
   </colors>
@@ -586,9 +660,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -652,12 +726,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
@@ -668,7 +742,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -695,10 +769,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -937,17 +1011,17 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1225,7 +1299,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1252,10 +1326,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1497,17 +1571,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="7.8125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="53.2344" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53.2109" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.8125" style="1" customWidth="1"/>
     <col min="4" max="4" width="35.8125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.6016" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6016" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.6016" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1520,721 +1595,819 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" ht="39" customHeight="1">
-      <c r="A3" s="6">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" t="s" s="10">
         <v>5</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" ht="27" customHeight="1">
-      <c r="A4" s="6">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="B4" t="s" s="10">
         <v>6</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" ht="27" customHeight="1">
-      <c r="A5" s="6">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="B5" t="s" s="10">
         <v>7</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" ht="27" customHeight="1">
-      <c r="A6" s="6">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="B6" t="s" s="10">
         <v>8</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" ht="39" customHeight="1">
-      <c r="A7" s="6">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" t="s" s="7">
+      <c r="B7" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" ht="27" customHeight="1">
-      <c r="A8" s="6">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" t="s" s="7">
+      <c r="B8" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" ht="39" customHeight="1">
-      <c r="A9" s="6">
+      <c r="A9" s="9">
         <v>7</v>
       </c>
-      <c r="B9" t="s" s="7">
+      <c r="B9" t="s" s="10">
         <v>11</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" ht="27" customHeight="1">
-      <c r="A10" s="6">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" t="s" s="7">
+      <c r="B10" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="C10" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s" s="14">
+        <v>14</v>
+      </c>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" ht="27" customHeight="1">
-      <c r="A11" s="6">
+      <c r="A11" s="9">
         <v>9</v>
       </c>
-      <c r="B11" t="s" s="7">
+      <c r="B11" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" ht="27" customHeight="1">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s" s="13">
         <v>13</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" ht="27" customHeight="1">
-      <c r="A12" s="6">
+      <c r="D12" t="s" s="14">
+        <v>17</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" ht="27" customHeight="1">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" ht="27" customHeight="1">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" ht="27" customHeight="1">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s" s="10">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" ht="27" customHeight="1">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" ht="39" customHeight="1">
+      <c r="A19" s="9">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" ht="39" customHeight="1">
+      <c r="A20" s="9">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s" s="10">
+        <v>26</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" ht="27" customHeight="1">
+      <c r="A21" s="9">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" ht="39" customHeight="1">
+      <c r="A22" s="9">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" ht="27" customHeight="1">
+      <c r="A23" s="9">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" ht="27" customHeight="1">
+      <c r="A24" s="9">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s" s="10">
+        <v>30</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" ht="63" customHeight="1">
+      <c r="A25" s="9">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s" s="10">
+        <v>31</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" ht="39" customHeight="1">
+      <c r="A26" s="9">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s" s="10">
+        <v>32</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" ht="27" customHeight="1">
+      <c r="A27" s="9">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" ht="27" customHeight="1">
+      <c r="A28" s="9">
         <v>10</v>
       </c>
-      <c r="B12" t="s" s="7">
+      <c r="B28" t="s" s="10">
+        <v>34</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" ht="27" customHeight="1">
+      <c r="A29" s="9">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" ht="27" customHeight="1">
+      <c r="A30" s="9">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" ht="27" customHeight="1">
+      <c r="A31" s="9">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s" s="10">
+        <v>37</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" ht="27" customHeight="1">
+      <c r="A32" s="9">
         <v>14</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="6">
+      <c r="B32" t="s" s="10">
+        <v>38</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" ht="15" customHeight="1">
+      <c r="A33" s="9">
+        <v>15</v>
+      </c>
+      <c r="B33" t="s" s="10">
+        <v>39</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" ht="27" customHeight="1">
+      <c r="A34" s="9">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s" s="10">
+        <v>40</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" ht="27" customHeight="1">
+      <c r="A35" s="9">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" ht="15" customHeight="1">
+      <c r="A36" t="s" s="15">
+        <v>42</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" ht="27" customHeight="1">
+      <c r="A37" s="9">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" ht="27" customHeight="1">
+      <c r="A38" s="9">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s" s="10">
+        <v>44</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" ht="27" customHeight="1">
+      <c r="A39" s="9">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s" s="10">
+        <v>45</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" ht="27" customHeight="1">
+      <c r="A40" s="9">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s" s="10">
+        <v>46</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" ht="15" customHeight="1">
+      <c r="A41" t="s" s="15">
+        <v>47</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" ht="27" customHeight="1">
+      <c r="A42" s="9">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s" s="10">
+        <v>48</v>
+      </c>
+      <c r="C42" s="11"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" ht="27" customHeight="1">
+      <c r="A43" s="9">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s" s="10">
+        <v>49</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="8"/>
+    </row>
+    <row r="44" ht="27" customHeight="1">
+      <c r="A44" s="9">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s" s="10">
+        <v>50</v>
+      </c>
+      <c r="C44" s="11"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" ht="15" customHeight="1">
+      <c r="A45" t="s" s="15">
+        <v>51</v>
+      </c>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" ht="27" customHeight="1">
+      <c r="A46" s="9">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s" s="10">
+        <v>52</v>
+      </c>
+      <c r="C46" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" ht="39" customHeight="1">
+      <c r="A47" s="9">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s" s="10">
+        <v>54</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" ht="27" customHeight="1">
+      <c r="A48" s="9">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s" s="10">
+        <v>55</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" ht="39" customHeight="1">
+      <c r="A49" s="9">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s" s="10">
+        <v>56</v>
+      </c>
+      <c r="C49" s="11"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="8"/>
+    </row>
+    <row r="50" ht="39" customHeight="1">
+      <c r="A50" s="9">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s" s="10">
+        <v>57</v>
+      </c>
+      <c r="C50" s="11"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" ht="39" customHeight="1">
+      <c r="A51" s="9">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" ht="27" customHeight="1">
+      <c r="A52" s="9">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s" s="10">
+        <v>59</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" ht="39" customHeight="1">
+      <c r="A53" s="9">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s" s="10">
+        <v>60</v>
+      </c>
+      <c r="C53" s="11"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" ht="39" customHeight="1">
+      <c r="A54" s="9">
+        <v>9</v>
+      </c>
+      <c r="B54" t="s" s="10">
+        <v>61</v>
+      </c>
+      <c r="C54" s="11"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" ht="27" customHeight="1">
+      <c r="A55" s="9">
+        <v>10</v>
+      </c>
+      <c r="B55" t="s" s="10">
+        <v>62</v>
+      </c>
+      <c r="C55" s="11"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" ht="27" customHeight="1">
+      <c r="A56" s="9">
         <v>11</v>
       </c>
-      <c r="B13" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" ht="27" customHeight="1">
-      <c r="A14" s="6">
+      <c r="B56" t="s" s="10">
+        <v>63</v>
+      </c>
+      <c r="C56" s="11"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" ht="27" customHeight="1">
+      <c r="A57" s="9">
         <v>12</v>
       </c>
-      <c r="B14" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" ht="27" customHeight="1">
-      <c r="A15" s="6">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" ht="27" customHeight="1">
-      <c r="A16" s="6">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" ht="27" customHeight="1">
-      <c r="A17" s="6">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" ht="39" customHeight="1">
-      <c r="A19" s="6">
+      <c r="B57" t="s" s="10">
+        <v>64</v>
+      </c>
+      <c r="C57" s="11"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="8"/>
+    </row>
+    <row r="58" ht="15" customHeight="1">
+      <c r="A58" t="s" s="15">
+        <v>65</v>
+      </c>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59" ht="39" customHeight="1">
+      <c r="A59" s="9">
         <v>1</v>
       </c>
-      <c r="B19" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" ht="39" customHeight="1">
-      <c r="A20" s="6">
+      <c r="B59" t="s" s="10">
+        <v>66</v>
+      </c>
+      <c r="C59" s="11"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60" ht="39" customHeight="1">
+      <c r="A60" s="9">
         <v>2</v>
       </c>
-      <c r="B20" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" ht="27" customHeight="1">
-      <c r="A21" s="6">
+      <c r="B60" t="s" s="10">
+        <v>67</v>
+      </c>
+      <c r="C60" s="11"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="8"/>
+    </row>
+    <row r="61" ht="51" customHeight="1">
+      <c r="A61" s="9">
         <v>3</v>
       </c>
-      <c r="B21" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" ht="39" customHeight="1">
-      <c r="A22" s="6">
+      <c r="B61" t="s" s="10">
+        <v>68</v>
+      </c>
+      <c r="C61" s="11"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="8"/>
+    </row>
+    <row r="62" ht="39" customHeight="1">
+      <c r="A62" s="9">
         <v>4</v>
       </c>
-      <c r="B22" t="s" s="7">
-        <v>24</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" ht="27" customHeight="1">
-      <c r="A23" s="6">
+      <c r="B62" t="s" s="10">
+        <v>69</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="8"/>
+    </row>
+    <row r="63" ht="39" customHeight="1">
+      <c r="A63" s="9">
         <v>5</v>
       </c>
-      <c r="B23" t="s" s="7">
-        <v>25</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" ht="27" customHeight="1">
-      <c r="A24" s="6">
+      <c r="B63" t="s" s="10">
+        <v>70</v>
+      </c>
+      <c r="C63" s="11"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="8"/>
+    </row>
+    <row r="64" ht="39" customHeight="1">
+      <c r="A64" s="9">
         <v>6</v>
       </c>
-      <c r="B24" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" ht="63" customHeight="1">
-      <c r="A25" s="6">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s" s="7">
-        <v>27</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" ht="39" customHeight="1">
-      <c r="A26" s="6">
-        <v>8</v>
-      </c>
-      <c r="B26" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" ht="27" customHeight="1">
-      <c r="A27" s="6">
-        <v>9</v>
-      </c>
-      <c r="B27" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" ht="27" customHeight="1">
-      <c r="A28" s="6">
-        <v>10</v>
-      </c>
-      <c r="B28" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" ht="27" customHeight="1">
-      <c r="A29" s="6">
-        <v>11</v>
-      </c>
-      <c r="B29" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" ht="27" customHeight="1">
-      <c r="A30" s="6">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" ht="27" customHeight="1">
-      <c r="A31" s="6">
-        <v>13</v>
-      </c>
-      <c r="B31" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" ht="27" customHeight="1">
-      <c r="A32" s="6">
-        <v>14</v>
-      </c>
-      <c r="B32" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" ht="15" customHeight="1">
-      <c r="A33" s="6">
-        <v>15</v>
-      </c>
-      <c r="B33" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="34" ht="27" customHeight="1">
-      <c r="A34" s="6">
-        <v>16</v>
-      </c>
-      <c r="B34" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" ht="27" customHeight="1">
-      <c r="A35" s="6">
-        <v>17</v>
-      </c>
-      <c r="B35" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" ht="15" customHeight="1">
-      <c r="A36" t="s" s="9">
-        <v>38</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-    </row>
-    <row r="37" ht="27" customHeight="1">
-      <c r="A37" s="6">
+      <c r="B64" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="C64" s="11"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="8"/>
+    </row>
+    <row r="65" ht="15" customHeight="1">
+      <c r="A65" t="s" s="15">
+        <v>72</v>
+      </c>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="8"/>
+    </row>
+    <row r="66" ht="15" customHeight="1">
+      <c r="A66" t="s" s="17">
+        <v>73</v>
+      </c>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" ht="51" customHeight="1">
+      <c r="A67" s="9">
         <v>1</v>
       </c>
-      <c r="B37" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-    </row>
-    <row r="38" ht="27" customHeight="1">
-      <c r="A38" s="6">
+      <c r="B67" t="s" s="10">
+        <v>74</v>
+      </c>
+      <c r="C67" s="11"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="8"/>
+    </row>
+    <row r="68" ht="27" customHeight="1">
+      <c r="A68" s="9">
         <v>2</v>
       </c>
-      <c r="B38" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-    </row>
-    <row r="39" ht="27" customHeight="1">
-      <c r="A39" s="6">
+      <c r="B68" t="s" s="10">
+        <v>75</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="8"/>
+    </row>
+    <row r="69" ht="51" customHeight="1">
+      <c r="A69" s="9">
         <v>3</v>
       </c>
-      <c r="B39" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-    </row>
-    <row r="40" ht="27" customHeight="1">
-      <c r="A40" s="6">
+      <c r="B69" t="s" s="10">
+        <v>76</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="8"/>
+    </row>
+    <row r="70" ht="39" customHeight="1">
+      <c r="A70" s="9">
         <v>4</v>
       </c>
-      <c r="B40" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-    </row>
-    <row r="41" ht="15" customHeight="1">
-      <c r="A41" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-    </row>
-    <row r="42" ht="27" customHeight="1">
-      <c r="A42" s="6">
+      <c r="B70" t="s" s="10">
+        <v>77</v>
+      </c>
+      <c r="C70" s="11"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="8"/>
+    </row>
+    <row r="71" ht="15" customHeight="1">
+      <c r="A71" t="s" s="17">
+        <v>78</v>
+      </c>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="8"/>
+    </row>
+    <row r="72" ht="27" customHeight="1">
+      <c r="A72" s="9">
         <v>1</v>
       </c>
-      <c r="B42" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-    </row>
-    <row r="43" ht="27" customHeight="1">
-      <c r="A43" s="6">
+      <c r="B72" t="s" s="10">
+        <v>79</v>
+      </c>
+      <c r="C72" s="11"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" ht="39" customHeight="1">
+      <c r="A73" s="9">
         <v>2</v>
       </c>
-      <c r="B43" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-    </row>
-    <row r="44" ht="27" customHeight="1">
-      <c r="A44" s="6">
+      <c r="B73" t="s" s="10">
+        <v>80</v>
+      </c>
+      <c r="C73" s="11"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="8"/>
+    </row>
+    <row r="74" ht="39" customHeight="1">
+      <c r="A74" s="9">
         <v>3</v>
       </c>
-      <c r="B44" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-    </row>
-    <row r="45" ht="15" customHeight="1">
-      <c r="A45" t="s" s="9">
-        <v>47</v>
-      </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-    </row>
-    <row r="46" ht="27" customHeight="1">
-      <c r="A46" s="6">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-    </row>
-    <row r="47" ht="39" customHeight="1">
-      <c r="A47" s="6">
-        <v>2</v>
-      </c>
-      <c r="B47" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-    </row>
-    <row r="48" ht="27" customHeight="1">
-      <c r="A48" s="6">
-        <v>3</v>
-      </c>
-      <c r="B48" t="s" s="7">
-        <v>50</v>
-      </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-    </row>
-    <row r="49" ht="39" customHeight="1">
-      <c r="A49" s="6">
-        <v>4</v>
-      </c>
-      <c r="B49" t="s" s="7">
-        <v>51</v>
-      </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-    </row>
-    <row r="50" ht="39" customHeight="1">
-      <c r="A50" s="6">
-        <v>5</v>
-      </c>
-      <c r="B50" t="s" s="7">
-        <v>52</v>
-      </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-    </row>
-    <row r="51" ht="39" customHeight="1">
-      <c r="A51" s="6">
-        <v>6</v>
-      </c>
-      <c r="B51" t="s" s="7">
-        <v>53</v>
-      </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-    </row>
-    <row r="52" ht="27" customHeight="1">
-      <c r="A52" s="6">
-        <v>7</v>
-      </c>
-      <c r="B52" t="s" s="7">
-        <v>54</v>
-      </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-    </row>
-    <row r="53" ht="39" customHeight="1">
-      <c r="A53" s="6">
-        <v>8</v>
-      </c>
-      <c r="B53" t="s" s="7">
-        <v>55</v>
-      </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-    </row>
-    <row r="54" ht="39" customHeight="1">
-      <c r="A54" s="6">
-        <v>9</v>
-      </c>
-      <c r="B54" t="s" s="7">
-        <v>56</v>
-      </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-    </row>
-    <row r="55" ht="27" customHeight="1">
-      <c r="A55" s="6">
-        <v>10</v>
-      </c>
-      <c r="B55" t="s" s="7">
-        <v>57</v>
-      </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-    </row>
-    <row r="56" ht="27" customHeight="1">
-      <c r="A56" s="6">
-        <v>11</v>
-      </c>
-      <c r="B56" t="s" s="7">
-        <v>58</v>
-      </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-    </row>
-    <row r="57" ht="27" customHeight="1">
-      <c r="A57" s="6">
-        <v>12</v>
-      </c>
-      <c r="B57" t="s" s="7">
-        <v>59</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-    </row>
-    <row r="58" ht="15" customHeight="1">
-      <c r="A58" t="s" s="9">
-        <v>60</v>
-      </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-    </row>
-    <row r="59" ht="39" customHeight="1">
-      <c r="A59" s="6">
-        <v>1</v>
-      </c>
-      <c r="B59" t="s" s="7">
-        <v>61</v>
-      </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-    </row>
-    <row r="60" ht="39" customHeight="1">
-      <c r="A60" s="6">
-        <v>2</v>
-      </c>
-      <c r="B60" t="s" s="7">
-        <v>62</v>
-      </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-    </row>
-    <row r="61" ht="51" customHeight="1">
-      <c r="A61" s="6">
-        <v>3</v>
-      </c>
-      <c r="B61" t="s" s="7">
-        <v>63</v>
-      </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-    </row>
-    <row r="62" ht="39" customHeight="1">
-      <c r="A62" s="6">
-        <v>4</v>
-      </c>
-      <c r="B62" t="s" s="7">
-        <v>64</v>
-      </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-    </row>
-    <row r="63" ht="39" customHeight="1">
-      <c r="A63" s="6">
-        <v>5</v>
-      </c>
-      <c r="B63" t="s" s="7">
-        <v>65</v>
-      </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-    </row>
-    <row r="64" ht="39" customHeight="1">
-      <c r="A64" s="6">
-        <v>6</v>
-      </c>
-      <c r="B64" t="s" s="7">
-        <v>66</v>
-      </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-    </row>
-    <row r="65" ht="15" customHeight="1">
-      <c r="A65" t="s" s="9">
-        <v>67</v>
-      </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-    </row>
-    <row r="66" ht="15" customHeight="1">
-      <c r="A66" t="s" s="11">
-        <v>68</v>
-      </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="13"/>
-    </row>
-    <row r="67" ht="51" customHeight="1">
-      <c r="A67" s="6">
-        <v>1</v>
-      </c>
-      <c r="B67" t="s" s="7">
-        <v>69</v>
-      </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-    </row>
-    <row r="68" ht="27" customHeight="1">
-      <c r="A68" s="6">
-        <v>2</v>
-      </c>
-      <c r="B68" t="s" s="7">
-        <v>70</v>
-      </c>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-    </row>
-    <row r="69" ht="51" customHeight="1">
-      <c r="A69" s="6">
-        <v>3</v>
-      </c>
-      <c r="B69" t="s" s="7">
-        <v>71</v>
-      </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-    </row>
-    <row r="70" ht="39" customHeight="1">
-      <c r="A70" s="6">
-        <v>4</v>
-      </c>
-      <c r="B70" t="s" s="7">
-        <v>72</v>
-      </c>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-    </row>
-    <row r="71" ht="15" customHeight="1">
-      <c r="A71" t="s" s="11">
-        <v>73</v>
-      </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="13"/>
-    </row>
-    <row r="72" ht="27" customHeight="1">
-      <c r="A72" s="6">
-        <v>1</v>
-      </c>
-      <c r="B72" t="s" s="7">
-        <v>74</v>
-      </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-    </row>
-    <row r="73" ht="39" customHeight="1">
-      <c r="A73" s="6">
-        <v>2</v>
-      </c>
-      <c r="B73" t="s" s="7">
-        <v>75</v>
-      </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-    </row>
-    <row r="74" ht="39" customHeight="1">
-      <c r="A74" s="6">
-        <v>3</v>
-      </c>
-      <c r="B74" t="s" s="7">
-        <v>76</v>
-      </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
+      <c r="B74" t="s" s="10">
+        <v>81</v>
+      </c>
+      <c r="C74" s="11"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>